<commit_message>
Fixed reading headers with empty cells
</commit_message>
<xml_diff>
--- a/test/datasets/testsets.xlsx
+++ b/test/datasets/testsets.xlsx
@@ -14,14 +14,15 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="dates" sheetId="2" r:id="rId2"/>
-    <sheet name="sharedstrings" sheetId="3" r:id="rId3"/>
+    <sheet name="booleans" sheetId="4" r:id="rId3"/>
+    <sheet name="sharedstrings" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Dates</t>
   </si>
@@ -58,6 +59,27 @@
   </si>
   <si>
     <t>3co.l</t>
+  </si>
+  <si>
+    <t>boolcol</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>moredata</t>
   </si>
 </sst>
 </file>
@@ -588,9 +610,87 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3:E8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="3" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C4" t="b">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C5" t="b">
+        <v>0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C6" t="b">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C7" t="b">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C8" t="b">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>

</xml_diff>